<commit_message>
mimhor changes added to requirements_testing_2
</commit_message>
<xml_diff>
--- a/requirements_testing/requirements_testing_2.xlsx
+++ b/requirements_testing/requirements_testing_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORK &amp; STUDY\WORK\git_resume\requirements_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7326332-1299-43D2-A8C9-C976C1D19403}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E835299-B9A7-42D3-B1CF-5440A0C927C4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -141,9 +141,6 @@
 Система должна быть ограничена только описанными функциями?</t>
   </si>
   <si>
-    <t>Требование неоднозначное, т.к. не указано, в виде какого элемента интерфейса веб-страницы должна быть отображена информация о названии сервиса. Требование неполное, т. к. не указано, где и как именно должен отображаться данный элемент.</t>
-  </si>
-  <si>
     <t>На главной странице должна присутствовать картинка с телефоном и 4 активные кнопки: Add Customer, Add Tariff Plan, Add Tariff Plan to Customer, Pay Billing и Delete Customer, а также описание для каждой из них. На данный момент оно выполнено в виде текста-филлера (Lorem ipsum...), но в следующих релизах будет обновлено</t>
   </si>
   <si>
@@ -158,15 +155,7 @@
     <t>Требование неполное, т. к. не указано, где именно под шапкой отображается название страницы Add Customer. Какие характеристики у текста в данном названии?</t>
   </si>
   <si>
-    <t xml:space="preserve">Требование неоднозначное, потому что не указано, где и как именно должны отображаться данные картинка, кнопки и описания. Как именно выглядит картинка? 
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Требование неоднозначное, т. к. неясно, о каком "боковом меню" идет речь? Имеется в виду "гамбургер-меню"? Какую именно кнопку "X" нужно использовать для закрытия данного меню? Можно ли использовать "X" на физической клавиатуре компьютера? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Требование неоднозначное, т. к. неясно, какими элементами интерфейса веб-страницы являются сущности "Background Check", "Pending", "Done". Можно выбрать один из трех данных элементов? Какие и где именно они должны отображаться?
-Требование противоречивое. Почему сущность "Done" означает то, что пользователь создан, если для создания пользователя нужно заполнить требуемые поля и кликнуть на кнопку "Submit" в тестируемой форме? </t>
   </si>
   <si>
     <t>Требование неоднозначное, т. к. неясно, каким элементом интерфейса является сущность "Billing Addres". Правильно ли указано его название? Где и как именно данный элемент отображается? Куда вводить First Name, Last Name, Email, Address и Mobile Number?</t>
@@ -204,6 +193,17 @@
 Требование неоднозначное.
 Как и где должно отображаться сообщение "Last Name must not be blank"? Каким элементом является данная сущность?
 Действительно ли необходимы именно такие сообщения о невалидных данных? Либо можно обойтись меньшим количеством более общих по смыслу сообщений о том, какие данные валидные?</t>
+  </si>
+  <si>
+    <t>Требование неполное, т.к. не указано, в виде какого элемента интерфейса веб-страницы должна быть отображена информация о названии сервиса. Где и как именно должен отображаться данный элемент?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Требование неполное, потому что не указано, где и как именно должны отображаться данные картинка, кнопки и описания. Как именно выглядит картинка? 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Требование неполное, неоднозначное, т. к. неясно, какими элементами интерфейса веб-страницы являются сущности "Background Check", "Pending", "Done". Можно выбрать один из трех данных элементов? Какие и где именно они должны отображаться?
+Требование противоречивое. Почему сущность "Done" означает то, что пользователь создан, если для создания пользователя нужно заполнить требуемые поля и кликнуть на кнопку "Submit" в тестируемой форме? </t>
   </si>
 </sst>
 </file>
@@ -582,8 +582,8 @@
   </sheetPr>
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -833,7 +833,7 @@
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
     </row>
-    <row r="9" spans="1:27" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="79.2" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>2</v>
       </c>
@@ -841,7 +841,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -872,10 +872,10 @@
         <v>3</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -909,7 +909,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -977,7 +977,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1041,7 +1041,7 @@
         <v>10</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1075,7 +1075,7 @@
         <v>11</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1109,7 +1109,7 @@
         <v>12</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1143,7 +1143,7 @@
         <v>13</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -1177,7 +1177,7 @@
         <v>14</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1211,7 +1211,7 @@
         <v>15</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1313,7 +1313,7 @@
         <v>20</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -1347,7 +1347,7 @@
         <v>21</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1446,7 +1446,7 @@
         <v>25</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -1481,7 +1481,7 @@
         <v>26</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -1516,7 +1516,7 @@
         <v>27</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1551,7 +1551,7 @@
         <v>28</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>

</xml_diff>